<commit_message>
COGMENTO-1238 Working on Contacts class it's in progress saved all contact elements
</commit_message>
<xml_diff>
--- a/src/main/resources/contactData/CogmentoTestData.xlsx
+++ b/src/main/resources/contactData/CogmentoTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="15020" tabRatio="500"/>
+    <workbookView windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="333">
   <si>
     <t>firstname</t>
   </si>
@@ -209,7 +209,7 @@
     <t>Some Identifier</t>
   </si>
   <si>
-    <t>src/main/resources/images/image.png</t>
+    <t>src/main/resources/images/1.png</t>
   </si>
   <si>
     <t>John</t>
@@ -668,7 +668,7 @@
     <t>March</t>
   </si>
   <si>
-    <t>src/main/resources/images/7.jpg</t>
+    <t>src/main/resources/images/1.jpg</t>
   </si>
   <si>
     <t>Sweeney</t>
@@ -721,9 +721,6 @@
     <t>Data scientist</t>
   </si>
   <si>
-    <t>src/main/resources/images/8.jpg</t>
-  </si>
-  <si>
     <t>Christina</t>
   </si>
   <si>
@@ -780,9 +777,6 @@
     <t>September</t>
   </si>
   <si>
-    <t>src/main/resources/images/9.jpg</t>
-  </si>
-  <si>
     <t>Britney</t>
   </si>
   <si>
@@ -833,9 +827,6 @@
     <t>Computer scientist</t>
   </si>
   <si>
-    <t>src/main/resources/images/10.jpg</t>
-  </si>
-  <si>
     <t>Spacey</t>
   </si>
   <si>
@@ -886,9 +877,6 @@
     <t>Cloud system engineer</t>
   </si>
   <si>
-    <t>src/main/resources/images/11.jpg</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
@@ -942,9 +930,6 @@
     <t>April</t>
   </si>
   <si>
-    <t>src/main/resources/images/12.jpg</t>
-  </si>
-  <si>
     <t>Uma</t>
   </si>
   <si>
@@ -1001,9 +986,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>src/main/resources/images/13.jpg</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -1060,9 +1042,6 @@
     <t>February</t>
   </si>
   <si>
-    <t>src/main/resources/images/14.jpg</t>
-  </si>
-  <si>
     <t>Morgan</t>
   </si>
   <si>
@@ -1116,9 +1095,6 @@
     <t>Applications engineer</t>
   </si>
   <si>
-    <t>src/main/resources/images/15.jpg</t>
-  </si>
-  <si>
     <t>Deni</t>
   </si>
   <si>
@@ -1169,9 +1145,6 @@
     <t>15555</t>
   </si>
   <si>
-    <t>src/main/resources/images/16.jpg</t>
-  </si>
-  <si>
     <t>Haruki</t>
   </si>
   <si>
@@ -1219,9 +1192,6 @@
     <t>16666</t>
   </si>
   <si>
-    <t>src/main/resources/images/17.jpg</t>
-  </si>
-  <si>
     <t>Lev</t>
   </si>
   <si>
@@ -1272,9 +1242,6 @@
     <t>17777</t>
   </si>
   <si>
-    <t>src/main/resources/images/18.jpg</t>
-  </si>
-  <si>
     <t>Dmitri</t>
   </si>
   <si>
@@ -1325,9 +1292,6 @@
     <t>18888</t>
   </si>
   <si>
-    <t>src/main/resources/images/19.jpg</t>
-  </si>
-  <si>
     <t>Smith</t>
   </si>
   <si>
@@ -1375,9 +1339,6 @@
     <t>19999</t>
   </si>
   <si>
-    <t>src/main/resources/images/20.jpg</t>
-  </si>
-  <si>
     <t>cal</t>
   </si>
 </sst>
@@ -1387,8 +1348,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -1417,33 +1378,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1454,44 +1392,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1507,17 +1417,39 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1529,9 +1461,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,6 +1478,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1553,10 +1499,25 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1569,31 +1530,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1611,7 +1584,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1623,13 +1662,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,19 +1680,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1665,91 +1698,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1793,15 +1754,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1817,26 +1769,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1858,6 +1795,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1867,11 +1815,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1880,134 +1841,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2362,8 +2323,8 @@
   <sheetPr/>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0078125" defaultRowHeight="14"/>
@@ -3378,21 +3339,21 @@
         <v>62</v>
       </c>
       <c r="AJ9" s="8" t="s">
-        <v>194</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
@@ -3401,7 +3362,7 @@
         <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>96</v>
@@ -3413,28 +3374,28 @@
         <v>98</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N10" s="2">
         <v>8</v>
       </c>
       <c r="O10" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>78</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>52</v>
@@ -3449,10 +3410,10 @@
         <v>128</v>
       </c>
       <c r="W10" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="Y10" s="2" t="s">
         <v>130</v>
@@ -3479,7 +3440,7 @@
         <v>31</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AH10" s="2">
         <v>1973</v>
@@ -3488,21 +3449,21 @@
         <v>62</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>208</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
@@ -3511,7 +3472,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>43</v>
@@ -3523,28 +3484,28 @@
         <v>121</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N11" s="2">
         <v>8</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>52</v>
@@ -3559,7 +3520,7 @@
         <v>54</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>149</v>
@@ -3598,7 +3559,7 @@
         <v>62</v>
       </c>
       <c r="AJ11" s="8" t="s">
-        <v>220</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -3606,13 +3567,13 @@
         <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>40</v>
@@ -3621,7 +3582,7 @@
         <v>180</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>70</v>
@@ -3633,28 +3594,28 @@
         <v>141</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N12" s="2">
         <v>8</v>
       </c>
       <c r="O12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="R12" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>52</v>
@@ -3669,10 +3630,10 @@
         <v>54</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>56</v>
@@ -3708,21 +3669,21 @@
         <v>62</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
@@ -3731,7 +3692,7 @@
         <v>193</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>96</v>
@@ -3743,25 +3704,25 @@
         <v>161</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>74</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N13" s="2">
         <v>8</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>104</v>
@@ -3779,10 +3740,10 @@
         <v>54</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>83</v>
@@ -3809,7 +3770,7 @@
         <v>12</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="AH13" s="2">
         <v>1972</v>
@@ -3818,30 +3779,30 @@
         <v>62</v>
       </c>
       <c r="AJ13" s="8" t="s">
-        <v>245</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>43</v>
@@ -3853,28 +3814,28 @@
         <v>45</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="N14" s="2">
         <v>8</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>52</v>
@@ -3889,7 +3850,7 @@
         <v>106</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>82</v>
@@ -3919,7 +3880,7 @@
         <v>26</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AH14" s="2">
         <v>1959</v>
@@ -3928,30 +3889,30 @@
         <v>62</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>259</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>70</v>
@@ -3963,28 +3924,28 @@
         <v>72</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N15" s="2">
         <v>8</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>52</v>
@@ -3999,10 +3960,10 @@
         <v>128</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y15" s="2" t="s">
         <v>130</v>
@@ -4029,7 +3990,7 @@
         <v>27</v>
       </c>
       <c r="AG15" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH15" s="2">
         <v>1983</v>
@@ -4038,30 +3999,30 @@
         <v>62</v>
       </c>
       <c r="AJ15" s="8" t="s">
-        <v>273</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>96</v>
@@ -4073,28 +4034,28 @@
         <v>98</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="N16" s="2">
         <v>8</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>52</v>
@@ -4109,7 +4070,7 @@
         <v>54</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>149</v>
@@ -4148,30 +4109,30 @@
         <v>62</v>
       </c>
       <c r="AJ16" s="2" t="s">
-        <v>286</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>43</v>
@@ -4183,28 +4144,28 @@
         <v>121</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="N17" s="2">
         <v>8</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>52</v>
@@ -4222,7 +4183,7 @@
         <v>41</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>56</v>
@@ -4249,7 +4210,7 @@
         <v>19</v>
       </c>
       <c r="AG17" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AH17" s="2">
         <v>1995</v>
@@ -4258,30 +4219,30 @@
         <v>62</v>
       </c>
       <c r="AJ17" s="8" t="s">
-        <v>298</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>70</v>
@@ -4293,28 +4254,28 @@
         <v>141</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="N18" s="2">
         <v>8</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>52</v>
@@ -4332,7 +4293,7 @@
         <v>68</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y18" s="2" t="s">
         <v>83</v>
@@ -4368,30 +4329,30 @@
         <v>62</v>
       </c>
       <c r="AJ18" s="2" t="s">
-        <v>309</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>43</v>
@@ -4403,28 +4364,28 @@
         <v>161</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="N19" s="2">
         <v>8</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>52</v>
@@ -4469,7 +4430,7 @@
         <v>3</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH19" s="2">
         <v>1970</v>
@@ -4478,30 +4439,30 @@
         <v>62</v>
       </c>
       <c r="AJ19" s="8" t="s">
-        <v>321</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="3" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>70</v>
@@ -4513,28 +4474,28 @@
         <v>45</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="N20" s="2">
         <v>8</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>52</v>
@@ -4552,7 +4513,7 @@
         <v>118</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y20" s="2" t="s">
         <v>130</v>
@@ -4588,7 +4549,7 @@
         <v>62</v>
       </c>
       <c r="AJ20" s="2" t="s">
-        <v>333</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:36">
@@ -4596,22 +4557,22 @@
         <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>96</v>
@@ -4623,28 +4584,28 @@
         <v>45</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="N21" s="2">
         <v>8</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>52</v>
@@ -4689,7 +4650,7 @@
         <v>21</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH21" s="2">
         <v>1972</v>
@@ -4698,7 +4659,7 @@
         <v>62</v>
       </c>
       <c r="AJ21" s="8" t="s">
-        <v>344</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4746,7 +4707,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
COGMENTO-1245 working on companies page
</commit_message>
<xml_diff>
--- a/src/main/resources/contactData/CogmentoTestData.xlsx
+++ b/src/main/resources/contactData/CogmentoTestData.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="14700" tabRatio="500"/>
+    <workbookView windowHeight="14740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="calls" sheetId="2" r:id="rId2"/>
     <sheet name="calendar" sheetId="3" r:id="rId3"/>
     <sheet name="documents" sheetId="4" r:id="rId4"/>
+    <sheet name="companies" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="373">
   <si>
     <t>run</t>
   </si>
@@ -1350,23 +1351,143 @@
   <si>
     <t>cal</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Phone Number Type</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Email Type</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Social Channels</t>
+  </si>
+  <si>
+    <t>Channels Handle</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Num of Employes</t>
+  </si>
+  <si>
+    <t>Stock Symbol</t>
+  </si>
+  <si>
+    <t>Annual Revenue</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>TechCenture Academy</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>https://techcenture.com</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>techcentureacademy@gmail.com</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>@TechCentureAcademy</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>src/main/resources/images/image.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1376,10 +1497,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1387,18 +1510,24 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9.75"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1411,44 +1540,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1456,30 +1548,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1494,6 +1562,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1501,14 +1608,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1524,9 +1631,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1551,30 +1680,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1593,19 +1698,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1617,7 +1716,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1635,13 +1800,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1653,61 +1830,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1719,7 +1848,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1748,15 +1877,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1768,6 +1888,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1787,6 +1916,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1798,6 +1936,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1820,28 +1969,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1850,145 +1979,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1996,19 +2146,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="48" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2332,145 +2482,145 @@
   <sheetPr/>
   <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0078125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="7.9609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.96875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.2265625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.65625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="36.9375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6171875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.1796875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.8984375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.40625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.4375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.4375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6171875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.4375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="15.71875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="21.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.7734375" style="1" customWidth="1"/>
-    <col min="36" max="36" width="17.4296875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="32.8671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.9609375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.96875" style="8" customWidth="1"/>
+    <col min="4" max="5" width="9.7265625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="6.328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.2265625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.65625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="36.9375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="13.6171875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="24.1796875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="13.8984375" style="8" customWidth="1"/>
+    <col min="16" max="16" width="14.40625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="11.4375" style="8" customWidth="1"/>
+    <col min="20" max="20" width="12.4375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="11.6171875" style="8" customWidth="1"/>
+    <col min="23" max="23" width="10.4375" style="8" customWidth="1"/>
+    <col min="24" max="24" width="15.71875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" style="8" customWidth="1"/>
+    <col min="28" max="28" width="11.7734375" style="8" customWidth="1"/>
+    <col min="36" max="36" width="17.4296875" style="8" customWidth="1"/>
+    <col min="37" max="37" width="32.8671875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2478,112 +2628,112 @@
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="9">
         <v>8</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="9">
         <v>22102</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AD2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AF2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AG2" s="9">
         <v>17</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AH2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="9">
         <v>1950</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AK2" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2591,112 +2741,112 @@
       <c r="A3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="9">
         <v>8</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="U3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="Z3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AB3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AD3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AE3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AF3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AG3" s="9">
         <v>12</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AH3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3" s="9">
         <v>1998</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AK3" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2704,112 +2854,112 @@
       <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="9">
         <v>8</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="U4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="X4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Y4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="Z4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AB4" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AC4" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AD4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AE4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AF4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AG4" s="9">
         <v>5</v>
       </c>
-      <c r="AH4" s="2" t="s">
+      <c r="AH4" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4" s="9">
         <v>1970</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AJ4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK4" s="2" t="s">
+      <c r="AK4" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2817,112 +2967,112 @@
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="9">
         <v>8</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="U5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Y5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="Z5" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AB5" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AC5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AD5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AE5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AF5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AG5" s="9">
         <v>11</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AH5" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AI5" s="9">
         <v>1991</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" s="15" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2930,112 +3080,112 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="9">
         <v>8</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="U6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="Z6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AC6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AD6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AE6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AF6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AG6" s="9">
         <v>15</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AH6" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AI6" s="9">
         <v>1971</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AJ6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AK6" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3043,112 +3193,112 @@
       <c r="A7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="9">
         <v>8</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R7" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="U7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="X7" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="Z7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AB7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AC7" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AD7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AE7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF7" s="2" t="s">
+      <c r="AF7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AG7" s="9">
         <v>19</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AH7" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AI7" s="9">
         <v>1992</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AJ7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK7" s="8" t="s">
+      <c r="AK7" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3156,112 +3306,112 @@
       <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="9">
         <v>8</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V8" s="3" t="s">
+      <c r="V8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="W8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="X8" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Y8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="Z8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AB8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AC8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AD8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AE8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AF8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AG8" s="9">
         <v>22</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AH8" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AI8" s="9">
         <v>1972</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AJ8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK8" s="2" t="s">
+      <c r="AK8" s="9" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3269,112 +3419,112 @@
       <c r="A9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="9">
         <v>8</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="Q9" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="R9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="U9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V9" s="3" t="s">
+      <c r="V9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="X9" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Y9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="Z9" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AB9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AC9" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AD9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AE9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AF9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AG9" s="9">
         <v>19</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AH9" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="AI9" s="9">
         <v>1993</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AJ9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK9" s="8" t="s">
+      <c r="AK9" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3382,112 +3532,112 @@
       <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="9">
         <v>8</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q10" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="S10" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="U10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V10" s="3" t="s">
+      <c r="V10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Y10" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AB10" s="2" t="s">
+      <c r="AB10" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AC10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AD10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AE10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AF10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="AG10" s="9">
         <v>31</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AH10" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="AI10" s="2">
+      <c r="AI10" s="9">
         <v>1973</v>
       </c>
-      <c r="AJ10" s="2" t="s">
+      <c r="AJ10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AK10" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3495,112 +3645,112 @@
       <c r="A11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="9">
         <v>8</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="Q11" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="R11" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="U11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V11" s="3" t="s">
+      <c r="V11" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="X11" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="Y11" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z11" s="2" t="s">
+      <c r="Z11" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA11" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AB11" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AC11" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AD11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AE11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AF11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="AG11" s="9">
         <v>5</v>
       </c>
-      <c r="AH11" s="2" t="s">
+      <c r="AH11" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="AI11" s="2">
+      <c r="AI11" s="9">
         <v>1965</v>
       </c>
-      <c r="AJ11" s="2" t="s">
+      <c r="AJ11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK11" s="8" t="s">
+      <c r="AK11" s="15" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3608,112 +3758,112 @@
       <c r="A12" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="9">
         <v>8</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="Q12" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="R12" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="S12" s="3" t="s">
+      <c r="S12" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="U12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V12" s="3" t="s">
+      <c r="V12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="W12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="X12" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Y12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="Z12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AA12" s="2" t="s">
+      <c r="AA12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AB12" s="2" t="s">
+      <c r="AB12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AC12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AD12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AE12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF12" s="2" t="s">
+      <c r="AF12" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG12" s="2">
+      <c r="AG12" s="9">
         <v>3</v>
       </c>
-      <c r="AH12" s="2" t="s">
+      <c r="AH12" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AI12" s="9">
         <v>1958</v>
       </c>
-      <c r="AJ12" s="2" t="s">
+      <c r="AJ12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK12" s="2" t="s">
+      <c r="AK12" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3721,112 +3871,112 @@
       <c r="A13" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="9">
         <v>8</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="R13" s="3" t="s">
+      <c r="R13" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="S13" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V13" s="3" t="s">
+      <c r="V13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="W13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="X13" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Y13" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="Z13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AA13" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AB13" s="2" t="s">
+      <c r="AB13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AC13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AD13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AE13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF13" s="2" t="s">
+      <c r="AF13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AG13" s="9">
         <v>12</v>
       </c>
-      <c r="AH13" s="2" t="s">
+      <c r="AH13" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AI13" s="9">
         <v>1972</v>
       </c>
-      <c r="AJ13" s="2" t="s">
+      <c r="AJ13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK13" s="8" t="s">
+      <c r="AK13" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3834,112 +3984,112 @@
       <c r="A14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="9">
         <v>8</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="R14" s="3" t="s">
+      <c r="R14" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="S14" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="U14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="V14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="W14" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="X14" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Y14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="Z14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AA14" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AB14" s="2" t="s">
+      <c r="AB14" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="AC14" s="2" t="s">
+      <c r="AC14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AD14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AE14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF14" s="2" t="s">
+      <c r="AF14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="AG14" s="9">
         <v>26</v>
       </c>
-      <c r="AH14" s="2" t="s">
+      <c r="AH14" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="AI14" s="9">
         <v>1959</v>
       </c>
-      <c r="AJ14" s="2" t="s">
+      <c r="AJ14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK14" s="2" t="s">
+      <c r="AK14" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3947,112 +4097,112 @@
       <c r="A15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="9">
         <v>8</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="Q15" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="R15" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="S15" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="T15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="U15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V15" s="3" t="s">
+      <c r="V15" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="W15" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="X15" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="Y15" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="Z15" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AA15" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AB15" s="2" t="s">
+      <c r="AB15" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AC15" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AD15" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AE15" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF15" s="2" t="s">
+      <c r="AF15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AG15" s="9">
         <v>27</v>
       </c>
-      <c r="AH15" s="2" t="s">
+      <c r="AH15" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AI15" s="9">
         <v>1983</v>
       </c>
-      <c r="AJ15" s="2" t="s">
+      <c r="AJ15" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK15" s="8" t="s">
+      <c r="AK15" s="15" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4060,112 +4210,112 @@
       <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="9">
         <v>8</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="R16" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="S16" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="T16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="U16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V16" s="3" t="s">
+      <c r="V16" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="W16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="X16" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="Y16" s="8" t="s">
+      <c r="Y16" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z16" s="2" t="s">
+      <c r="Z16" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="AB16" s="2" t="s">
+      <c r="AB16" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AC16" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AD16" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AE16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF16" s="2" t="s">
+      <c r="AF16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AG16" s="9">
         <v>25</v>
       </c>
-      <c r="AH16" s="2" t="s">
+      <c r="AH16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI16" s="9">
         <v>1987</v>
       </c>
-      <c r="AJ16" s="2" t="s">
+      <c r="AJ16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AK16" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4173,112 +4323,112 @@
       <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="9">
         <v>8</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P17" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="R17" s="3" t="s">
+      <c r="R17" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="S17" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="U17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V17" s="3" t="s">
+      <c r="V17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="W17" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="X17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Y17" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="Z17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AA17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AB17" s="2" t="s">
+      <c r="AB17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AC17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AD17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AE17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF17" s="2" t="s">
+      <c r="AF17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG17" s="2">
+      <c r="AG17" s="9">
         <v>19</v>
       </c>
-      <c r="AH17" s="2" t="s">
+      <c r="AH17" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="AI17" s="2">
+      <c r="AI17" s="9">
         <v>1995</v>
       </c>
-      <c r="AJ17" s="2" t="s">
+      <c r="AJ17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK17" s="8" t="s">
+      <c r="AK17" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4286,112 +4436,112 @@
       <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="9">
         <v>8</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="P18" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="Q18" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="R18" s="3" t="s">
+      <c r="R18" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S18" s="3" t="s">
+      <c r="S18" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="U18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V18" s="3" t="s">
+      <c r="V18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="W18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="X18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Y18" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="Z18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AA18" s="2" t="s">
+      <c r="AA18" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AB18" s="2" t="s">
+      <c r="AB18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AC18" s="2" t="s">
+      <c r="AC18" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AD18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE18" s="2" t="s">
+      <c r="AE18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF18" s="2" t="s">
+      <c r="AF18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AG18" s="2">
+      <c r="AG18" s="9">
         <v>7</v>
       </c>
-      <c r="AH18" s="2" t="s">
+      <c r="AH18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AI18" s="2">
+      <c r="AI18" s="9">
         <v>1992</v>
       </c>
-      <c r="AJ18" s="2" t="s">
+      <c r="AJ18" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK18" s="2" t="s">
+      <c r="AK18" s="9" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4399,112 +4549,112 @@
       <c r="A19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="9">
         <v>8</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="P19" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="Q19" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="R19" s="3" t="s">
+      <c r="R19" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="S19" s="3" t="s">
+      <c r="S19" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="T19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="U19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V19" s="3" t="s">
+      <c r="V19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="W19" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="X19" s="2" t="s">
+      <c r="X19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="Y19" s="2" t="s">
+      <c r="Y19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Z19" s="2" t="s">
+      <c r="Z19" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AA19" s="2" t="s">
+      <c r="AA19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AB19" s="2" t="s">
+      <c r="AB19" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="AC19" s="2" t="s">
+      <c r="AC19" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AD19" s="2" t="s">
+      <c r="AD19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AE19" s="2" t="s">
+      <c r="AE19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF19" s="2" t="s">
+      <c r="AF19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG19" s="2">
+      <c r="AG19" s="9">
         <v>3</v>
       </c>
-      <c r="AH19" s="2" t="s">
+      <c r="AH19" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="AI19" s="2">
+      <c r="AI19" s="9">
         <v>1970</v>
       </c>
-      <c r="AJ19" s="2" t="s">
+      <c r="AJ19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK19" s="8" t="s">
+      <c r="AK19" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4512,112 +4662,112 @@
       <c r="A20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L20" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N20" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="9">
         <v>8</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="P20" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="Q20" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="R20" s="3" t="s">
+      <c r="R20" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="S20" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="U20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V20" s="3" t="s">
+      <c r="V20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="W20" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="X20" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="Y20" s="2" t="s">
+      <c r="Y20" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="Z20" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="AA20" s="2" t="s">
+      <c r="AA20" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AB20" s="2" t="s">
+      <c r="AB20" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AC20" s="2" t="s">
+      <c r="AC20" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AD20" s="2" t="s">
+      <c r="AD20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE20" s="2" t="s">
+      <c r="AE20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AF20" s="2" t="s">
+      <c r="AF20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG20" s="2">
+      <c r="AG20" s="9">
         <v>8</v>
       </c>
-      <c r="AH20" s="2" t="s">
+      <c r="AH20" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AI20" s="2">
+      <c r="AI20" s="9">
         <v>1985</v>
       </c>
-      <c r="AJ20" s="2" t="s">
+      <c r="AJ20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK20" s="2" t="s">
+      <c r="AK20" s="9" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4625,112 +4775,112 @@
       <c r="A21" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="L21" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21" s="9">
         <v>8</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="P21" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q21" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="R21" s="3" t="s">
+      <c r="R21" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="S21" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="U21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V21" s="3" t="s">
+      <c r="V21" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="W21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="X21" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="Y21" s="8" t="s">
+      <c r="Y21" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="Z21" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="AA21" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="AB21" s="2" t="s">
+      <c r="AB21" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AC21" s="2" t="s">
+      <c r="AC21" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AD21" s="2" t="s">
+      <c r="AD21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AE21" s="2" t="s">
+      <c r="AE21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AF21" s="2" t="s">
+      <c r="AF21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AG21" s="2">
+      <c r="AG21" s="9">
         <v>21</v>
       </c>
-      <c r="AH21" s="2" t="s">
+      <c r="AH21" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="AI21" s="2">
+      <c r="AI21" s="9">
         <v>1972</v>
       </c>
-      <c r="AJ21" s="2" t="s">
+      <c r="AJ21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AK21" s="8" t="s">
+      <c r="AK21" s="15" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4778,7 +4928,7 @@
   <sheetFormatPr defaultColWidth="9.0078125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4821,4 +4971,237 @@
   <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AF2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="7.1875" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
+    <col min="5" max="5" width="13.5625" customWidth="1"/>
+    <col min="6" max="6" width="7.1875" customWidth="1"/>
+    <col min="7" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="9" max="10" width="12.4375" customWidth="1"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="12" width="18.5625" customWidth="1"/>
+    <col min="13" max="13" width="29.4375" customWidth="1"/>
+    <col min="14" max="14" width="10.125" customWidth="1"/>
+    <col min="15" max="15" width="5.375" customWidth="1"/>
+    <col min="17" max="17" width="14.5625" customWidth="1"/>
+    <col min="18" max="18" width="21.5" customWidth="1"/>
+    <col min="19" max="19" width="7.875" customWidth="1"/>
+    <col min="20" max="20" width="16" customWidth="1"/>
+    <col min="21" max="21" width="12.75" customWidth="1"/>
+    <col min="22" max="22" width="14.75" customWidth="1"/>
+    <col min="23" max="23" width="6.9375" customWidth="1"/>
+    <col min="24" max="24" width="6.5625" customWidth="1"/>
+    <col min="25" max="25" width="7.5" customWidth="1"/>
+    <col min="26" max="26" width="6.125" customWidth="1"/>
+    <col min="27" max="27" width="7.5625" customWidth="1"/>
+    <col min="28" max="28" width="9.5" customWidth="1"/>
+    <col min="29" max="29" width="33.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="3">
+        <v>22132</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2026547833</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="T2" s="5">
+        <v>120</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="V2" s="6">
+        <v>700000</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>12983455</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" display="techcentureacademy@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://techcenture.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>